<commit_message>
Begin and Beneficiary Completed with testing
</commit_message>
<xml_diff>
--- a/System 6 Related Information/BOTL Segment Definition.xlsx
+++ b/System 6 Related Information/BOTL Segment Definition.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="240" windowWidth="18780" windowHeight="8130" activeTab="2"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3655" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3655" uniqueCount="569">
   <si>
     <t>Tag</t>
   </si>
@@ -1758,6 +1758,12 @@
   </si>
   <si>
     <t>This is the ID of the product/package being upgraded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t xml:space="preserve">string  </t>
   </si>
 </sst>
 </file>
@@ -2296,6 +2302,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2352,10 +2359,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I352"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10653,10 +10661,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="B334" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11979,10 +11988,10 @@
         <v>123</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>124</v>
+        <v>567</v>
       </c>
       <c r="E54" s="8">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>125</v>
@@ -13240,10 +13249,10 @@
         <v>220</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>221</v>
+        <v>567</v>
       </c>
       <c r="E109" s="11">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F109" s="11" t="s">
         <v>222</v>
@@ -15402,10 +15411,10 @@
         <v>398</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>399</v>
+        <v>568</v>
       </c>
       <c r="E197" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F197" s="8" t="s">
         <v>400</v>
@@ -15427,10 +15436,10 @@
         <v>401</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>399</v>
+        <v>567</v>
       </c>
       <c r="E198" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F198" s="8" t="s">
         <v>402</v>
@@ -15452,10 +15461,10 @@
         <v>403</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>399</v>
+        <v>567</v>
       </c>
       <c r="E199" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F199" s="8" t="s">
         <v>404</v>
@@ -15799,10 +15808,10 @@
         <v>431</v>
       </c>
       <c r="D214" s="11" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="E214" s="11">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="F214" s="11" t="s">
         <v>432</v>

</xml_diff>